<commit_message>
excel test - sheet to objectarray
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/OpenEmrData.xlsx
+++ b/src/test/resources/testdata/OpenEmrData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JiDi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\B-Mine\Company\Company\Scientific Games2\java_selenium_workspace\OpenEmrApplication\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -32,31 +32,31 @@
     <t>Password</t>
   </si>
   <si>
+    <t>admin123</t>
+  </si>
+  <si>
+    <t>English (Indian)</t>
+  </si>
+  <si>
+    <t>Invalid usernama and password</t>
+  </si>
+  <si>
+    <t>john</t>
+  </si>
+  <si>
+    <t>john123</t>
+  </si>
+  <si>
+    <t>bala</t>
+  </si>
+  <si>
+    <t>Dutch</t>
+  </si>
+  <si>
     <t>Language</t>
   </si>
   <si>
-    <t>ExpectedValue</t>
-  </si>
-  <si>
-    <t>admin123</t>
-  </si>
-  <si>
-    <t>pass</t>
-  </si>
-  <si>
-    <t>English (Indian)</t>
-  </si>
-  <si>
-    <t>Invalid usernama and password</t>
-  </si>
-  <si>
-    <t>john</t>
-  </si>
-  <si>
-    <t>john123</t>
-  </si>
-  <si>
-    <t>Dutch</t>
+    <t>expectedValue</t>
   </si>
 </sst>
 </file>
@@ -377,7 +377,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A4" sqref="A4:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -396,38 +396,38 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
         <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dataproviderutils with excel connect for invalidcredentialtest
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/OpenEmrData.xlsx
+++ b/src/test/resources/testdata/OpenEmrData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>Username</t>
   </si>
@@ -38,9 +38,6 @@
     <t>English (Indian)</t>
   </si>
   <si>
-    <t>Invalid usernama and password</t>
-  </si>
-  <si>
     <t>john</t>
   </si>
   <si>
@@ -57,6 +54,15 @@
   </si>
   <si>
     <t>expectedValue</t>
+  </si>
+  <si>
+    <t>Invalid username or password</t>
+  </si>
+  <si>
+    <t>bala123</t>
+  </si>
+  <si>
+    <t>Invalid username or password123</t>
   </si>
 </sst>
 </file>
@@ -374,10 +380,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD1048576"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -396,10 +402,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
         <v>9</v>
-      </c>
-      <c r="D1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -407,27 +413,41 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>4</v>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
day 4- xml parameterization
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/OpenEmrData.xlsx
+++ b/src/test/resources/testdata/OpenEmrData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>Username</t>
   </si>
@@ -60,9 +60,6 @@
   </si>
   <si>
     <t>bala123</t>
-  </si>
-  <si>
-    <t>Invalid username or password123</t>
   </si>
 </sst>
 </file>
@@ -447,7 +444,7 @@
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>